<commit_message>
Update on 20241107 part 3
</commit_message>
<xml_diff>
--- a/各地组播源汇总/新疆.xlsx
+++ b/各地组播源汇总/新疆.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3787" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3797" uniqueCount="588">
   <si>
     <t>电信组播</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1789,6 +1789,14 @@
   </si>
   <si>
     <t>IPB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/udp/238.125.1.34:5140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新视觉</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2135,7 +2143,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E757"/>
+  <dimension ref="A1:E759"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -15015,6 +15023,40 @@
       </c>
       <c r="E757" t="s">
         <v>429</v>
+      </c>
+    </row>
+    <row r="758" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A758" t="s">
+        <v>587</v>
+      </c>
+      <c r="B758" t="s">
+        <v>572</v>
+      </c>
+      <c r="C758" t="s">
+        <v>573</v>
+      </c>
+      <c r="D758" t="s">
+        <v>574</v>
+      </c>
+      <c r="E758" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="759" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A759" t="s">
+        <v>587</v>
+      </c>
+      <c r="B759" t="s">
+        <v>572</v>
+      </c>
+      <c r="C759" t="s">
+        <v>573</v>
+      </c>
+      <c r="D759" t="s">
+        <v>585</v>
+      </c>
+      <c r="E759" t="s">
+        <v>586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>